<commit_message>
Version in use at the lake.
* After hooking up both sensors.
* After calibration.
* Adjusted display spacing to work for real-world values.
</commit_message>
<xml_diff>
--- a/hardware/voltage_divider_calcs.xlsx
+++ b/hardware/voltage_divider_calcs.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>R1</t>
   </si>
@@ -42,6 +42,9 @@
     <t>Calibrated Ratio for Arduino</t>
   </si>
   <si>
+    <t>Hardware</t>
+  </si>
+  <si>
     <t>Theory</t>
   </si>
   <si>
@@ -55,6 +58,21 @@
   </si>
   <si>
     <t>Divider 3</t>
+  </si>
+  <si>
+    <t>Long one</t>
+  </si>
+  <si>
+    <t>Divider 4</t>
+  </si>
+  <si>
+    <t>1: 30 V, 5 A</t>
+  </si>
+  <si>
+    <t>Divider 5</t>
+  </si>
+  <si>
+    <t>2: 30 V, 30 A</t>
   </si>
   <si>
     <t>Power Source</t>
@@ -100,6 +118,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -121,6 +140,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -195,10 +215,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -210,7 +230,8 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.6836734693878"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9030612244898"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -238,10 +259,13 @@
       <c r="I1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>107.3</v>
@@ -257,7 +281,7 @@
         <v>0.819050042408821</v>
       </c>
       <c r="F2" s="1" t="n">
-        <f aca="false"> 5 / C2 * (B2+C2)</f>
+        <f aca="false">5 / C2 * (B2+C2)</f>
         <v>55.6132075471698</v>
       </c>
       <c r="G2" s="1" t="n">
@@ -274,7 +298,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="n">
         <f aca="false">B2</f>
@@ -300,7 +324,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="n">
@@ -330,7 +354,7 @@
         <v>1.71303827535404</v>
       </c>
       <c r="F5" s="1" t="n">
-        <f aca="false"> 5 / C5 * (B5+C5)</f>
+        <f aca="false">5 / C5 * (B5+C5)</f>
         <v>26.5901822833387</v>
       </c>
       <c r="G5" s="1" t="n">
@@ -341,7 +365,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>609</v>
@@ -357,7 +381,7 @@
         <v>1.86719321148825</v>
       </c>
       <c r="F8" s="1" t="n">
-        <f aca="false"> 5 / C8 * (B8+C8)</f>
+        <f aca="false">5 / C8 * (B8+C8)</f>
         <v>24.3949044585987</v>
       </c>
       <c r="G8" s="1" t="n">
@@ -374,7 +398,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>610</v>
@@ -390,7 +414,7 @@
         <v>1.23479490806223</v>
       </c>
       <c r="F9" s="1" t="n">
-        <f aca="false"> 5 / C9 * (B9+C9)</f>
+        <f aca="false">5 / C9 * (B9+C9)</f>
         <v>36.4432989690722</v>
       </c>
       <c r="G9" s="1" t="n">
@@ -403,6 +427,79 @@
       </c>
       <c r="I9" s="0" t="n">
         <v>7.2497</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>610</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>8.96</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <f aca="false">5 / C10 * (B10+C10)</f>
+        <v>33.7735849056604</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <f aca="false">F10 * F10 / (B10+C10)</f>
+        <v>1.59309362762549</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <f aca="false">D10/E10</f>
+        <v>6.78787878787879</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>6.5277</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>552</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>8.96</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <f aca="false">5 / C11 * (B11+C11)</f>
+        <v>36.0112359550562</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <f aca="false">F11 * F11 / (B11+C11)</f>
+        <v>2.02310314354248</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <f aca="false">D11/E11</f>
+        <v>7.2258064516129</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>7.0797</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -423,7 +520,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -438,21 +535,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2.52</v>
@@ -460,7 +557,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2.54</v>
@@ -472,7 +569,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3.32</v>
@@ -484,7 +581,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
@@ -496,7 +593,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4.7</v>
@@ -506,13 +603,13 @@
         <v>4.36</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>